<commit_message>
update student from fill up class 6
</commit_message>
<xml_diff>
--- a/Copy of Class 6 Admission Info.xlsx
+++ b/Copy of Class 6 Admission Info.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOURAV TRADERS\Desktop\New folder\Study-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA6489C-AB37-4F6C-B156-9AF3C4F37CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991EDDA8-F34E-40C6-A928-763B7F4D4198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kulsum" sheetId="8" r:id="rId1"/>
-    <sheet name="Anamika" sheetId="7" r:id="rId2"/>
+    <sheet name="Nuri" sheetId="9" r:id="rId1"/>
+    <sheet name="Kulsum" sheetId="8" r:id="rId2"/>
     <sheet name="Sathi" sheetId="6" r:id="rId3"/>
-    <sheet name="Khushi" sheetId="5" r:id="rId4"/>
-    <sheet name="SUMAIYA" sheetId="3" r:id="rId5"/>
-    <sheet name="SHRABONTI" sheetId="2" r:id="rId6"/>
-    <sheet name="SISTY" sheetId="1" r:id="rId7"/>
+    <sheet name="Anamika" sheetId="7" r:id="rId4"/>
+    <sheet name="Khushi" sheetId="5" r:id="rId5"/>
+    <sheet name="SUMAIYA" sheetId="3" r:id="rId6"/>
+    <sheet name="SHRABONTI" sheetId="2" r:id="rId7"/>
+    <sheet name="SISTY" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>নাম</t>
   </si>
@@ -258,6 +259,36 @@
   </si>
   <si>
     <t>19947316431000306</t>
+  </si>
+  <si>
+    <t>01763299043</t>
+  </si>
+  <si>
+    <t>Nuri Akter</t>
+  </si>
+  <si>
+    <t>21-08-2012</t>
+  </si>
+  <si>
+    <t>20127316431041697</t>
+  </si>
+  <si>
+    <t>01346468836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nur mohammad </t>
+  </si>
+  <si>
+    <t>6448364239</t>
+  </si>
+  <si>
+    <t>mrs. Nasima Begum</t>
+  </si>
+  <si>
+    <t>4640446003</t>
+  </si>
+  <si>
+    <t>KANIAL KHATA munsipara</t>
   </si>
 </sst>
 </file>
@@ -601,11 +632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3127A75F-5342-4E22-A930-8C79E7C774EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9D7969-76D0-49F4-A9A4-CD0B585F3219}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,7 +709,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -683,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,208 +734,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E93F5B-7D30-4A45-8E2B-49E98FE50BBD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3127A75F-5342-4E22-A930-8C79E7C774EF}">
   <sheetPr>
-    <tabColor theme="0"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5925181-8068-449B-9E6B-D62E727451E3}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA26A98-C654-4C8F-A25F-1B9A335A0226}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -919,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -935,21 +771,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -985,6 +823,210 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5925181-8068-449B-9E6B-D62E727451E3}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E93F5B-7D30-4A45-8E2B-49E98FE50BBD}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -998,6 +1040,108 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA26A98-C654-4C8F-A25F-1B9A335A0226}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CDE8F7-FBE4-440B-952C-FE782903AC9E}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1099,7 +1243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFE5440-EE40-4B29-A7A4-4F9E310B018F}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1201,7 +1345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>

</xml_diff>